<commit_message>
US187994: add prof_ and dfa_ to collection names
</commit_message>
<xml_diff>
--- a/database/files/business-upload/department_upload_template.xlsx
+++ b/database/files/business-upload/department_upload_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\Documents\cisco\tasks\business upload\arindam\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\work\fin-dfa\database\files\business-upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,6 +78,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> will be </t>
     </r>
@@ -94,6 +95,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> from the source pull.</t>
     </r>
@@ -103,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -122,12 +124,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -229,7 +225,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -545,7 +541,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>